<commit_message>
Squashed commit of the following:
commit eb2b7d782a309adf2f2decc1b0ea7a393607ee79
Author: 1000Dat <166731709+1000Dat@users.noreply.github.com>
Date:   Wed Jun 26 23:29:35 2024 +0700

    upadate

commit 30e8f6571895df069719fd04be96906fdd443efc
Author: 1000Dat <166731709+1000Dat@users.noreply.github.com>
Date:   Tue Jun 25 02:02:20 2024 +0700

    update job
</commit_message>
<xml_diff>
--- a/InterviewManagement/src/main/resources/edited_template.xlsx
+++ b/InterviewManagement/src/main/resources/edited_template.xlsx
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Total Of Job</t>
   </si>
@@ -43,6 +43,15 @@
   </si>
   <si>
     <t>Number Of Fail</t>
+  </si>
+  <si>
+    <t>Errors:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Row 1: Trùng Title. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Row 2: Ngày bắt đầu không được là quá khứ. Định dạng ngày kết thúc không hợp lệ hoặc trống. Giá trị T không hợp lệ hoặc trống. </t>
   </si>
 </sst>
 </file>
@@ -395,7 +404,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF128B99-204C-48C7-815C-366214971B01}">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -423,6 +432,21 @@
         <v>2.0</v>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>